<commit_message>
added diagrams 12, 13 to finished diagrams, renamed old folder
</commit_message>
<xml_diff>
--- a/sequence_diagrams/finishedSequentialDiagrams.xlsx
+++ b/sequence_diagrams/finishedSequentialDiagrams.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="420" windowWidth="27555" windowHeight="12825" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25725" windowHeight="7245" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use-Case 1" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="Use-Case 13" sheetId="13" r:id="rId13"/>
     <sheet name="Use-Case 14" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:S22"/>
 </workbook>
 </file>
 
@@ -459,7 +459,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1169,12 +1169,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1213,6 +1207,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,8 +1223,121 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDA6FAF0-9671-4CD4-AA4F-7D99BB4AE6F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="10058400" cy="7772400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>569204</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74DFAF7C-873D-4B36-A370-C5C3396B0AEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6665204" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1270,7 +1383,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1303,9 +1416,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1338,6 +1468,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1513,7 +1660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA61"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -1539,38 +1686,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="F1" s="60" t="s">
+      <c r="D1" s="81"/>
+      <c r="F1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="81"/>
+      <c r="I1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="L1" s="60" t="s">
+      <c r="J1" s="81"/>
+      <c r="L1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="O1" s="60" t="s">
+      <c r="M1" s="81"/>
+      <c r="O1" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="61"/>
-      <c r="R1" s="60" t="s">
+      <c r="P1" s="81"/>
+      <c r="R1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="U1" s="60" t="s">
+      <c r="S1" s="81"/>
+      <c r="U1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="61"/>
-      <c r="X1" s="60" t="s">
+      <c r="V1" s="81"/>
+      <c r="X1" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="61"/>
+      <c r="Y1" s="81"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
@@ -3297,7 +3444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3309,7 +3456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3336,30 +3483,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="H1" s="60" t="s">
+      <c r="F1" s="81"/>
+      <c r="H1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="K1" s="60" t="s">
+      <c r="I1" s="81"/>
+      <c r="K1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="61"/>
-      <c r="N1" s="60" t="s">
+      <c r="L1" s="81"/>
+      <c r="N1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="61"/>
-      <c r="Q1" s="60" t="s">
+      <c r="O1" s="81"/>
+      <c r="Q1" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="R1" s="81"/>
+      <c r="T1" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="61"/>
+      <c r="U1" s="81"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E2" s="5"/>
@@ -4043,7 +4190,7 @@
       <c r="D28" s="9"/>
       <c r="E28" s="5"/>
       <c r="F28" s="29"/>
-      <c r="G28" s="62" t="s">
+      <c r="G28" s="60" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="9"/>
@@ -4416,19 +4563,34 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4436,26 +4598,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -4464,7 +4615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4488,30 +4639,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="F1" s="60" t="s">
+      <c r="D1" s="81"/>
+      <c r="F1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="81"/>
+      <c r="I1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="L1" s="60" t="s">
+      <c r="J1" s="81"/>
+      <c r="L1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="O1" s="60" t="s">
+      <c r="M1" s="81"/>
+      <c r="O1" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="61"/>
-      <c r="R1" s="60" t="s">
+      <c r="P1" s="81"/>
+      <c r="R1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="61"/>
+      <c r="S1" s="81"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
@@ -5453,7 +5604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5478,30 +5629,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="F1" s="60" t="s">
+      <c r="D1" s="81"/>
+      <c r="F1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="81"/>
+      <c r="I1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="L1" s="60" t="s">
+      <c r="J1" s="81"/>
+      <c r="L1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="P1" s="60" t="s">
+      <c r="M1" s="81"/>
+      <c r="P1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="61"/>
-      <c r="S1" s="60" t="s">
+      <c r="Q1" s="81"/>
+      <c r="S1" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="61"/>
+      <c r="T1" s="81"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
@@ -6508,7 +6659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6535,30 +6686,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="H1" s="60" t="s">
+      <c r="F1" s="81"/>
+      <c r="H1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="K1" s="60" t="s">
+      <c r="I1" s="81"/>
+      <c r="K1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="61"/>
-      <c r="N1" s="60" t="s">
+      <c r="L1" s="81"/>
+      <c r="N1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="61"/>
-      <c r="Q1" s="60" t="s">
+      <c r="O1" s="81"/>
+      <c r="Q1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="R1" s="81"/>
+      <c r="T1" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="61"/>
+      <c r="U1" s="81"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E2" s="5"/>
@@ -7242,7 +7393,7 @@
       <c r="D28" s="9"/>
       <c r="E28" s="5"/>
       <c r="F28" s="29"/>
-      <c r="G28" s="62" t="s">
+      <c r="G28" s="60" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="9"/>
@@ -7625,12 +7776,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -7638,10 +7789,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:U9"/>
     </sheetView>
   </sheetViews>
@@ -7664,30 +7815,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="F1" s="60" t="s">
+      <c r="D1" s="81"/>
+      <c r="F1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="81"/>
+      <c r="I1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="L1" s="60" t="s">
+      <c r="J1" s="81"/>
+      <c r="L1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="O1" s="60" t="s">
+      <c r="M1" s="81"/>
+      <c r="O1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="61"/>
-      <c r="R1" s="60" t="s">
+      <c r="P1" s="81"/>
+      <c r="R1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="61"/>
+      <c r="S1" s="81"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
@@ -8339,7 +8490,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="9"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="63" t="s">
+      <c r="H31" s="61" t="s">
         <v>82</v>
       </c>
       <c r="I31" s="9"/>
@@ -8396,7 +8547,7 @@
       <c r="N33" s="10"/>
       <c r="O33" s="9"/>
       <c r="P33" s="12"/>
-      <c r="Q33" s="64" t="s">
+      <c r="Q33" s="62" t="s">
         <v>89</v>
       </c>
       <c r="R33" s="5"/>
@@ -8421,7 +8572,7 @@
       <c r="N34" s="10"/>
       <c r="O34" s="9"/>
       <c r="P34" s="12"/>
-      <c r="Q34" s="65" t="s">
+      <c r="Q34" s="63" t="s">
         <v>90</v>
       </c>
       <c r="R34" s="5"/>
@@ -8468,7 +8619,7 @@
       <c r="K36" s="37"/>
       <c r="L36" s="35"/>
       <c r="M36" s="36"/>
-      <c r="N36" s="66" t="s">
+      <c r="N36" s="64" t="s">
         <v>86</v>
       </c>
       <c r="O36" s="9"/>
@@ -8888,19 +9039,19 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="O1:P1"/>
-    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8926,30 +9077,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="F1" s="60" t="s">
+      <c r="D1" s="81"/>
+      <c r="F1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="81"/>
+      <c r="I1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="L1" s="60" t="s">
+      <c r="J1" s="81"/>
+      <c r="L1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="P1" s="60" t="s">
+      <c r="M1" s="81"/>
+      <c r="P1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="61"/>
-      <c r="S1" s="60" t="s">
+      <c r="Q1" s="81"/>
+      <c r="S1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="61"/>
+      <c r="T1" s="81"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
@@ -9912,19 +10063,19 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9951,30 +10102,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="G1" s="60" t="s">
+      <c r="E1" s="81"/>
+      <c r="G1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="J1" s="60" t="s">
+      <c r="H1" s="81"/>
+      <c r="J1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="61"/>
-      <c r="M1" s="60" t="s">
+      <c r="K1" s="81"/>
+      <c r="M1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="P1" s="60" t="s">
+      <c r="N1" s="81"/>
+      <c r="P1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="61"/>
-      <c r="S1" s="60" t="s">
+      <c r="Q1" s="81"/>
+      <c r="S1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="61"/>
+      <c r="T1" s="81"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
@@ -10296,9 +10447,9 @@
       <c r="F17" s="10"/>
       <c r="G17" s="9"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="68"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="66"/>
       <c r="L17" s="50" t="s">
         <v>100</v>
       </c>
@@ -10502,25 +10653,25 @@
       <c r="B25" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="57"/>
-      <c r="G25" s="69"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="58"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="73" t="s">
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="S25" s="69"/>
+      <c r="S25" s="67"/>
       <c r="T25" s="58"/>
       <c r="U25" s="58"/>
       <c r="V25" s="58"/>
@@ -10673,7 +10824,7 @@
       <c r="O31" s="37"/>
       <c r="P31" s="35"/>
       <c r="Q31" s="36"/>
-      <c r="R31" s="66" t="s">
+      <c r="R31" s="64" t="s">
         <v>86</v>
       </c>
       <c r="S31" s="9"/>
@@ -11054,25 +11205,25 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
-      <c r="B46" s="77" t="s">
+      <c r="B46" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="71"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="69"/>
       <c r="F46" s="57"/>
-      <c r="G46" s="69"/>
+      <c r="G46" s="67"/>
       <c r="H46" s="58"/>
-      <c r="I46" s="78"/>
-      <c r="J46" s="78"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="80"/>
-      <c r="M46" s="80"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="81" t="s">
+      <c r="I46" s="76"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="78"/>
+      <c r="M46" s="78"/>
+      <c r="N46" s="78"/>
+      <c r="O46" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="P46" s="69"/>
+      <c r="P46" s="67"/>
       <c r="Q46" s="58"/>
       <c r="R46" s="57"/>
       <c r="S46" s="57"/>
@@ -11368,19 +11519,19 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11407,30 +11558,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="G1" s="60" t="s">
+      <c r="E1" s="81"/>
+      <c r="G1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="J1" s="60" t="s">
+      <c r="H1" s="81"/>
+      <c r="J1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="61"/>
-      <c r="M1" s="60" t="s">
+      <c r="K1" s="81"/>
+      <c r="M1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="P1" s="60" t="s">
+      <c r="N1" s="81"/>
+      <c r="P1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="61"/>
-      <c r="S1" s="60" t="s">
+      <c r="Q1" s="81"/>
+      <c r="S1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="61"/>
+      <c r="T1" s="81"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
@@ -11752,9 +11903,9 @@
       <c r="F17" s="10"/>
       <c r="G17" s="9"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="68"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="66"/>
       <c r="L17" s="50" t="s">
         <v>100</v>
       </c>
@@ -11958,25 +12109,25 @@
       <c r="B25" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="57"/>
-      <c r="G25" s="69"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="58"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="73" t="s">
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="S25" s="69"/>
+      <c r="S25" s="67"/>
       <c r="T25" s="58"/>
       <c r="U25" s="58"/>
       <c r="V25" s="58"/>
@@ -12129,7 +12280,7 @@
       <c r="O31" s="37"/>
       <c r="P31" s="35"/>
       <c r="Q31" s="36"/>
-      <c r="R31" s="66" t="s">
+      <c r="R31" s="64" t="s">
         <v>86</v>
       </c>
       <c r="S31" s="9"/>
@@ -12226,7 +12377,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="9"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="65"/>
+      <c r="I35" s="63"/>
       <c r="J35" s="9"/>
       <c r="K35" s="12"/>
       <c r="L35" s="10"/>
@@ -12431,25 +12582,25 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
-      <c r="B43" s="77" t="s">
+      <c r="B43" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="71"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="57"/>
-      <c r="G43" s="69"/>
+      <c r="G43" s="67"/>
       <c r="H43" s="58"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="78"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="80"/>
-      <c r="M43" s="80"/>
-      <c r="N43" s="80"/>
-      <c r="O43" s="81" t="s">
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="77"/>
+      <c r="L43" s="78"/>
+      <c r="M43" s="78"/>
+      <c r="N43" s="78"/>
+      <c r="O43" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="P43" s="69"/>
+      <c r="P43" s="67"/>
       <c r="Q43" s="58"/>
       <c r="R43" s="57"/>
       <c r="S43" s="57"/>
@@ -12745,19 +12896,19 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12784,30 +12935,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="H1" s="60" t="s">
+      <c r="F1" s="81"/>
+      <c r="H1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="K1" s="60" t="s">
+      <c r="I1" s="81"/>
+      <c r="K1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="61"/>
-      <c r="N1" s="60" t="s">
+      <c r="L1" s="81"/>
+      <c r="N1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="61"/>
-      <c r="Q1" s="60" t="s">
+      <c r="O1" s="81"/>
+      <c r="Q1" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="R1" s="81"/>
+      <c r="T1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="61"/>
+      <c r="U1" s="81"/>
       <c r="V1" s="21"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -13785,7 +13936,7 @@
       <c r="D38" s="9"/>
       <c r="E38" s="5"/>
       <c r="F38" s="29"/>
-      <c r="G38" s="62" t="s">
+      <c r="G38" s="60" t="s">
         <v>73</v>
       </c>
       <c r="H38" s="9"/>
@@ -14172,12 +14323,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>